<commit_message>
fix animation of error message in validator
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\MatSaiGon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0067225-F628-49A2-AB0A-E4A8263AD82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BDD48-5C01-44FD-B8E6-173EC42AFEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Element reference breaks on modification of innerHTML property of container (
 nextBtnCSL when commonservice add html, the var that refer to nextBtnCSL is no
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Validate trường input date</t>
+  </si>
+  <si>
+    <t>đã fix</t>
+  </si>
+  <si>
+    <t>Add and remove same css class instantly</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4363957/add-and-remove-same-css-class-instantly</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -546,12 +555,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -559,20 +568,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
fix validate date of modal form
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\MatSaiGon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BDD48-5C01-44FD-B8E6-173EC42AFEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A25AC83-48D1-444A-A03E-9A40E6CB0686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Element reference breaks on modification of innerHTML property of container (
 nextBtnCSL when commonservice add html, the var that refer to nextBtnCSL is no
@@ -470,7 +470,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -590,6 +590,9 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -601,8 +604,9 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{A6B4E859-1917-42E0-B4F7-F69B8BBC3D14}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{69E5A691-3C52-41EE-83B2-5ED9CD77CBAC}"/>
+    <hyperlink ref="B18" r:id="rId3" xr:uid="{953D94A6-8EDE-4576-BC2F-0CCA8C424029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>